<commit_message>
Added descriptions to scenarios
</commit_message>
<xml_diff>
--- a/simulation/scenarios.xlsx
+++ b/simulation/scenarios.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ej45/Documents/walrusCKMR/simulation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28635716-7FFB-E74C-A3CB-5C7E747D7209}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E616542-B116-C049-9E20-D26CED92EAF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6340" yWindow="740" windowWidth="23060" windowHeight="18380" xr2:uid="{E7FF8656-E179-2341-868A-AC1C3D505F19}"/>
+    <workbookView xWindow="4520" yWindow="500" windowWidth="23060" windowHeight="18380" activeTab="2" xr2:uid="{E7FF8656-E179-2341-868A-AC1C3D505F19}"/>
   </bookViews>
   <sheets>
     <sheet name="demography" sheetId="2" r:id="rId1"/>
     <sheet name="lethality" sheetId="3" r:id="rId2"/>
     <sheet name="sampling" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>Scenario</t>
   </si>
@@ -68,6 +68,48 @@
   </si>
   <si>
     <t>RoI</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Null</t>
+  </si>
+  <si>
+    <t>Stable</t>
+  </si>
+  <si>
+    <t>Decreasing</t>
+  </si>
+  <si>
+    <t>Increasing</t>
+  </si>
+  <si>
+    <t>Reality + 100% effort 2025-2026</t>
+  </si>
+  <si>
+    <t>Reality + 100% effort 2025-2027</t>
+  </si>
+  <si>
+    <t>Reality + 100% effort 2025-2028</t>
+  </si>
+  <si>
+    <t>Reality + 75% effort 2025-2026</t>
+  </si>
+  <si>
+    <t>100% effort 2023-2028</t>
+  </si>
+  <si>
+    <t>100% effort 2023-2025</t>
+  </si>
+  <si>
+    <t>Reality + 75% effort through 2028</t>
+  </si>
+  <si>
+    <t>Reality + 75% effort through 2027</t>
+  </si>
+  <si>
+    <t>Total Effort</t>
   </si>
 </sst>
 </file>
@@ -446,15 +488,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4DDF907-AEC9-C042-9130-F30069439BA1}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -482,8 +524,11 @@
       <c r="I1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -497,7 +542,7 @@
         <v>0.5</v>
       </c>
       <c r="E2">
-        <v>0.67</v>
+        <v>0.7</v>
       </c>
       <c r="F2">
         <v>0.9</v>
@@ -511,8 +556,11 @@
       <c r="I2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -540,8 +588,11 @@
       <c r="I3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -569,8 +620,11 @@
       <c r="I4">
         <v>-0.02</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -597,6 +651,9 @@
       </c>
       <c r="I5">
         <v>0.01</v>
+      </c>
+      <c r="J5" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -681,15 +738,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{670BCB0E-2067-CC45-A8D9-AD5C6A958C6D}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="8" max="8" width="27.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -711,8 +771,14 @@
       <c r="G1" s="1">
         <v>2028</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -734,8 +800,15 @@
       <c r="G2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2">
+        <f>SUM(B2:G2)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -757,8 +830,15 @@
       <c r="G3" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I9" si="0">SUM(B3:G3)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -780,8 +860,15 @@
       <c r="G4" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -803,8 +890,15 @@
       <c r="G5" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -826,8 +920,15 @@
       <c r="G6" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -849,8 +950,15 @@
       <c r="G7" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -872,8 +980,15 @@
       <c r="G8" s="1">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -894,6 +1009,13 @@
       </c>
       <c r="G9" s="1">
         <v>0</v>
+      </c>
+      <c r="H9" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated results, figures, and manuscript edits
</commit_message>
<xml_diff>
--- a/simulation/scenarios.xlsx
+++ b/simulation/scenarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ej45/Documents/walrusCKMR/simulation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E616542-B116-C049-9E20-D26CED92EAF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC80C1DE-276B-A044-B8F7-A8A5BD1E5AA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4520" yWindow="500" windowWidth="23060" windowHeight="18380" activeTab="2" xr2:uid="{E7FF8656-E179-2341-868A-AC1C3D505F19}"/>
+    <workbookView xWindow="1860" yWindow="740" windowWidth="23060" windowHeight="18380" activeTab="2" xr2:uid="{E7FF8656-E179-2341-868A-AC1C3D505F19}"/>
   </bookViews>
   <sheets>
     <sheet name="demography" sheetId="2" r:id="rId1"/>
@@ -741,7 +741,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H9"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Updated (final?!?!?!?) test results
</commit_message>
<xml_diff>
--- a/simulation/scenarios.xlsx
+++ b/simulation/scenarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ej45/Documents/walrusCKMR/simulation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC80C1DE-276B-A044-B8F7-A8A5BD1E5AA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF1DDFB-758D-A84C-8DF6-E97824A667B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="740" windowWidth="23060" windowHeight="18380" activeTab="2" xr2:uid="{E7FF8656-E179-2341-868A-AC1C3D505F19}"/>
+    <workbookView xWindow="13160" yWindow="1820" windowWidth="23060" windowHeight="18380" activeTab="1" xr2:uid="{E7FF8656-E179-2341-868A-AC1C3D505F19}"/>
   </bookViews>
   <sheets>
     <sheet name="demography" sheetId="2" r:id="rId1"/>
@@ -663,10 +663,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2012C410-7FD4-B243-87D1-CDE037FAAD59}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -729,6 +729,26 @@
       </c>
       <c r="F3">
         <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1000</v>
+      </c>
+      <c r="C4">
+        <v>1000</v>
+      </c>
+      <c r="D4">
+        <v>1000</v>
+      </c>
+      <c r="E4">
+        <v>1000</v>
+      </c>
+      <c r="F4">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>
@@ -740,7 +760,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{670BCB0E-2067-CC45-A8D9-AD5C6A958C6D}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
IDK what changed in here -- hopefully nothing
</commit_message>
<xml_diff>
--- a/simulation/scenarios.xlsx
+++ b/simulation/scenarios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ej45/Documents/walrusCKMR/simulation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF1DDFB-758D-A84C-8DF6-E97824A667B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC32EAC0-A969-9147-90AB-BAEC865D3D4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13160" yWindow="1820" windowWidth="23060" windowHeight="18380" activeTab="1" xr2:uid="{E7FF8656-E179-2341-868A-AC1C3D505F19}"/>
+    <workbookView xWindow="13160" yWindow="1820" windowWidth="23060" windowHeight="18380" activeTab="2" xr2:uid="{E7FF8656-E179-2341-868A-AC1C3D505F19}"/>
   </bookViews>
   <sheets>
     <sheet name="demography" sheetId="2" r:id="rId1"/>
@@ -97,9 +97,6 @@
     <t>Reality + 75% effort 2025-2026</t>
   </si>
   <si>
-    <t>100% effort 2023-2028</t>
-  </si>
-  <si>
     <t>100% effort 2023-2025</t>
   </si>
   <si>
@@ -110,6 +107,9 @@
   </si>
   <si>
     <t>Total Effort</t>
+  </si>
+  <si>
+    <t>100% effort 2023-2027</t>
   </si>
 </sst>
 </file>
@@ -665,7 +665,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2012C410-7FD4-B243-87D1-CDE037FAAD59}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -760,8 +760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{670BCB0E-2067-CC45-A8D9-AD5C6A958C6D}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -795,7 +795,7 @@
         <v>10</v>
       </c>
       <c r="I1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -818,14 +818,14 @@
         <v>1</v>
       </c>
       <c r="G2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="I2">
         <f>SUM(B2:G2)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -971,7 +971,7 @@
         <v>0</v>
       </c>
       <c r="H7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I7">
         <f t="shared" si="0"/>
@@ -1001,7 +1001,7 @@
         <v>0.75</v>
       </c>
       <c r="H8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I8">
         <f t="shared" si="0"/>
@@ -1031,7 +1031,7 @@
         <v>0</v>
       </c>
       <c r="H9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I9">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
scenarios modified to include extra lethal samples
</commit_message>
<xml_diff>
--- a/simulation/scenarios.xlsx
+++ b/simulation/scenarios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ej45/Documents/walrusCKMR/simulation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC32EAC0-A969-9147-90AB-BAEC865D3D4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3FE4A36-8D6A-864F-9B50-9418729F04AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13160" yWindow="1820" windowWidth="23060" windowHeight="18380" activeTab="2" xr2:uid="{E7FF8656-E179-2341-868A-AC1C3D505F19}"/>
+    <workbookView xWindow="6340" yWindow="740" windowWidth="23060" windowHeight="18380" activeTab="1" xr2:uid="{E7FF8656-E179-2341-868A-AC1C3D505F19}"/>
   </bookViews>
   <sheets>
     <sheet name="demography" sheetId="2" r:id="rId1"/>
@@ -491,7 +491,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="A5" sqref="A5:K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -663,9 +663,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2012C410-7FD4-B243-87D1-CDE037FAAD59}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -736,18 +736,38 @@
         <v>3</v>
       </c>
       <c r="B4">
+        <v>500</v>
+      </c>
+      <c r="C4">
+        <v>500</v>
+      </c>
+      <c r="D4">
+        <v>500</v>
+      </c>
+      <c r="E4">
+        <v>500</v>
+      </c>
+      <c r="F4">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
         <v>1000</v>
       </c>
-      <c r="C4">
+      <c r="C5">
         <v>1000</v>
       </c>
-      <c r="D4">
+      <c r="D5">
         <v>1000</v>
       </c>
-      <c r="E4">
+      <c r="E5">
         <v>1000</v>
       </c>
-      <c r="F4">
+      <c r="F5">
         <v>1000</v>
       </c>
     </row>
@@ -760,7 +780,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{670BCB0E-2067-CC45-A8D9-AD5C6A958C6D}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>

</xml_diff>